<commit_message>
created inst_impl_test as a main to test for the correctness when implementing instruction
</commit_message>
<xml_diff>
--- a/instructions.xlsx
+++ b/instructions.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomastang/Documents/imperial/year2/eieproject/local stuff/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomastang/Documents/imperial/year2/eieproject/arch2-2017-cw-Exception/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="18180" yWindow="440" windowWidth="15460" windowHeight="20560" tabRatio="500"/>
+    <workbookView xWindow="17120" yWindow="440" windowWidth="15460" windowHeight="20560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="59">
   <si>
     <t>ADD</t>
   </si>
@@ -198,23 +198,22 @@
   </si>
   <si>
     <t>X</t>
+  </si>
+  <si>
+    <t>Implementation?</t>
+  </si>
+  <si>
+    <t>COMPLEXITY</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -226,8 +225,23 @@
       <name val="Helvetica"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -240,17 +254,37 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="1"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -259,10 +293,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -540,457 +589,841 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D54"/>
+  <dimension ref="A1:F54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A58" sqref="A58"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.1640625" customWidth="1"/>
-    <col min="2" max="4" width="27.1640625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="13.5" customWidth="1"/>
+    <col min="2" max="4" width="6" style="2" customWidth="1"/>
+    <col min="5" max="5" width="22.5" customWidth="1"/>
+    <col min="6" max="6" width="16.1640625" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="E1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="E2" s="5">
+        <v>-1</v>
+      </c>
+      <c r="F2" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="E3" s="5">
+        <v>-1</v>
+      </c>
+      <c r="F3" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="E4" s="5">
+        <v>-1</v>
+      </c>
+      <c r="F4" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="E5" s="5">
+        <v>-1</v>
+      </c>
+      <c r="F5" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="E6" s="5">
+        <v>-1</v>
+      </c>
+      <c r="F6" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="E7" s="5">
+        <v>-1</v>
+      </c>
+      <c r="F7" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="E8" s="5">
+        <v>-1</v>
+      </c>
+      <c r="F8" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="E9" s="5">
+        <v>-1</v>
+      </c>
+      <c r="F9" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="E10" s="5">
+        <v>-1</v>
+      </c>
+      <c r="F10" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="E11" s="5">
+        <v>-1</v>
+      </c>
+      <c r="F11" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="E12" s="5">
+        <v>-1</v>
+      </c>
+      <c r="F12" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="E13" s="5">
+        <v>-1</v>
+      </c>
+      <c r="F13" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="E14" s="5">
+        <v>-1</v>
+      </c>
+      <c r="F14" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="E15" s="5">
+        <v>-1</v>
+      </c>
+      <c r="F15" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="E16" s="5">
+        <v>-1</v>
+      </c>
+      <c r="F16" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="E17" s="5">
+        <v>-1</v>
+      </c>
+      <c r="F17" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="E18" s="5">
+        <v>-1</v>
+      </c>
+      <c r="F18" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="E19" s="5">
+        <v>-1</v>
+      </c>
+      <c r="F19" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="E20" s="5">
+        <v>-1</v>
+      </c>
+      <c r="F20" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="E21" s="5">
+        <v>-1</v>
+      </c>
+      <c r="F21" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="E22" s="5">
+        <v>-1</v>
+      </c>
+      <c r="F22" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="E23" s="5">
+        <v>-1</v>
+      </c>
+      <c r="F23" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="E24" s="5">
+        <v>-1</v>
+      </c>
+      <c r="F24" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="E25" s="5">
+        <v>-1</v>
+      </c>
+      <c r="F25" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="E26" s="5">
+        <v>-1</v>
+      </c>
+      <c r="F26" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="E27" s="5">
+        <v>-1</v>
+      </c>
+      <c r="F27" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="E28" s="5">
+        <v>-1</v>
+      </c>
+      <c r="F28" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="E29" s="5">
+        <v>-1</v>
+      </c>
+      <c r="F29" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="E30" s="5">
+        <v>-1</v>
+      </c>
+      <c r="F30" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="E31" s="5">
+        <v>-1</v>
+      </c>
+      <c r="F31" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="E32" s="5">
+        <v>-1</v>
+      </c>
+      <c r="F32" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="E33" s="5">
+        <v>-1</v>
+      </c>
+      <c r="F33" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="E34" s="5">
+        <v>-1</v>
+      </c>
+      <c r="F34" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="E35" s="5">
+        <v>-1</v>
+      </c>
+      <c r="F35" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="E36" s="5">
+        <v>-1</v>
+      </c>
+      <c r="F36" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="E37" s="5">
+        <v>-1</v>
+      </c>
+      <c r="F37" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>36</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="E38" s="5">
+        <v>-1</v>
+      </c>
+      <c r="F38" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="E39" s="5">
+        <v>-1</v>
+      </c>
+      <c r="F39" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="E40" s="5">
+        <v>-1</v>
+      </c>
+      <c r="F40" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="E41" s="5">
+        <v>-1</v>
+      </c>
+      <c r="F41" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="E42" s="5">
+        <v>-1</v>
+      </c>
+      <c r="F42" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="E43" s="5">
+        <v>-1</v>
+      </c>
+      <c r="F43" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="E44" s="5">
+        <v>-1</v>
+      </c>
+      <c r="F44" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="E45" s="5">
+        <v>-1</v>
+      </c>
+      <c r="F45" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="E46" s="5">
+        <v>-1</v>
+      </c>
+      <c r="F46" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="E47" s="5">
+        <v>-1</v>
+      </c>
+      <c r="F47" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="E48" s="5">
+        <v>-1</v>
+      </c>
+      <c r="F48" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="E49" s="5">
+        <v>-1</v>
+      </c>
+      <c r="F49" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>48</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="E50" s="5">
+        <v>-1</v>
+      </c>
+      <c r="F50" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="E51" s="5">
+        <v>-1</v>
+      </c>
+      <c r="F51" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>50</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="E52" s="5">
+        <v>-1</v>
+      </c>
+      <c r="F52" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="E53" s="5">
+        <v>-1</v>
+      </c>
+      <c r="F53" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>52</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>56</v>
       </c>
+      <c r="E54" s="5">
+        <v>-1</v>
+      </c>
+      <c r="F54" s="7">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="E2:E54">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="formula" val="EXACT(no,$E$2:$E$54)"/>
+        <cfvo type="formula" val="EXACT(ok,$E$2:$E$54)"/>
+        <cfvo type="formula" val="EXACT(good,$E$2:$E$54)"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF92D050"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E54">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="num" val="-1"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF92D050"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1:F1048576">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="num" val="&quot;1,2&quot;"/>
+        <cfvo type="num" val="3"/>
+        <cfvo type="num" val="5"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:F54">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF92D050"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Implemented complexity 2 Instructions
-Implemented: ADDIU, ANDI, LUI, ORI, SLL, SLT, SRA, SRAV, SRL, XORI.

- ADD, ADDI, LW, SUB, SW not yet implemented (need memory and overflow function)
</commit_message>
<xml_diff>
--- a/instructions.xlsx
+++ b/instructions.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="15620" yWindow="440" windowWidth="16960" windowHeight="20500" tabRatio="500"/>
+    <workbookView xWindow="14880" yWindow="440" windowWidth="16960" windowHeight="20500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="63">
   <si>
     <t>ADD</t>
   </si>
@@ -213,6 +213,9 @@
   </si>
   <si>
     <t>still need to make sure exception break is working correctly,90% working</t>
+  </si>
+  <si>
+    <t>memory not yet implemented</t>
   </si>
 </sst>
 </file>
@@ -600,8 +603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.2"/>
@@ -672,7 +675,7 @@
         <v>56</v>
       </c>
       <c r="E4" s="5">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="F4" s="7">
         <v>2</v>
@@ -714,7 +717,7 @@
         <v>56</v>
       </c>
       <c r="E7" s="5">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="F7" s="7">
         <v>2</v>
@@ -983,7 +986,7 @@
         <v>56</v>
       </c>
       <c r="E26" s="5">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="F26" s="7">
         <v>2</v>
@@ -1002,6 +1005,9 @@
       <c r="F27" s="7">
         <v>2</v>
       </c>
+      <c r="G27" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
@@ -1137,7 +1143,7 @@
         <v>56</v>
       </c>
       <c r="E37" s="5">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="F37" s="7">
         <v>2</v>
@@ -1179,7 +1185,7 @@
         <v>56</v>
       </c>
       <c r="E40" s="5">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="F40" s="7">
         <v>2</v>
@@ -1207,7 +1213,7 @@
         <v>56</v>
       </c>
       <c r="E42" s="5">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="F42" s="7">
         <v>2</v>

</xml_diff>

<commit_message>
updated instruction excel sheet
</commit_message>
<xml_diff>
--- a/instructions.xlsx
+++ b/instructions.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="14880" yWindow="440" windowWidth="16960" windowHeight="20500" tabRatio="500"/>
+    <workbookView xWindow="19220" yWindow="440" windowWidth="11700" windowHeight="20500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="66">
   <si>
     <t>ADD</t>
   </si>
@@ -212,10 +212,19 @@
     <t>if result is "negative" SUBU does not raise overflow</t>
   </si>
   <si>
-    <t>still need to make sure exception break is working correctly,90% working</t>
-  </si>
-  <si>
     <t>memory not yet implemented</t>
+  </si>
+  <si>
+    <t>need to implement sub overflow</t>
+  </si>
+  <si>
+    <t>need to implement add overflow</t>
+  </si>
+  <si>
+    <t>read more on opcode</t>
+  </si>
+  <si>
+    <t>might have to check imm value</t>
   </si>
 </sst>
 </file>
@@ -603,8 +612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.2"/>
@@ -652,6 +661,9 @@
       <c r="F2" s="7">
         <v>2</v>
       </c>
+      <c r="G2" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -731,10 +743,13 @@
         <v>56</v>
       </c>
       <c r="E8" s="5">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="F8" s="7">
         <v>3</v>
+      </c>
+      <c r="G8" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -750,6 +765,9 @@
       <c r="F9" s="7">
         <v>3</v>
       </c>
+      <c r="G9" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -764,6 +782,9 @@
       <c r="F10" s="7">
         <v>4</v>
       </c>
+      <c r="G10" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -773,7 +794,7 @@
         <v>56</v>
       </c>
       <c r="E11" s="5">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="F11" s="7">
         <v>3</v>
@@ -787,7 +808,7 @@
         <v>56</v>
       </c>
       <c r="E12" s="5">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="F12" s="7">
         <v>3</v>
@@ -806,6 +827,9 @@
       <c r="F13" s="7">
         <v>3</v>
       </c>
+      <c r="G13" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -820,6 +844,9 @@
       <c r="F14" s="7">
         <v>4</v>
       </c>
+      <c r="G14" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -829,7 +856,7 @@
         <v>56</v>
       </c>
       <c r="E15" s="5">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="F15" s="7">
         <v>3</v>
@@ -843,7 +870,7 @@
         <v>56</v>
       </c>
       <c r="E16" s="5">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="F16" s="7">
         <v>4</v>
@@ -857,7 +884,7 @@
         <v>56</v>
       </c>
       <c r="E17" s="5">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="F17" s="7">
         <v>4</v>
@@ -871,7 +898,7 @@
         <v>56</v>
       </c>
       <c r="E18" s="5">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="F18" s="7">
         <v>3</v>
@@ -885,7 +912,7 @@
         <v>56</v>
       </c>
       <c r="E19" s="5">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="F19" s="7">
         <v>4</v>
@@ -899,7 +926,7 @@
         <v>56</v>
       </c>
       <c r="E20" s="5">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="F20" s="7">
         <v>4</v>
@@ -913,13 +940,10 @@
         <v>56</v>
       </c>
       <c r="E21" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F21" s="7">
         <v>1</v>
-      </c>
-      <c r="G21" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -935,6 +959,9 @@
       <c r="F22" s="7">
         <v>3</v>
       </c>
+      <c r="G22" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
@@ -949,6 +976,9 @@
       <c r="F23" s="7">
         <v>3</v>
       </c>
+      <c r="G23" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
@@ -963,6 +993,9 @@
       <c r="F24" s="7">
         <v>3</v>
       </c>
+      <c r="G24" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
@@ -977,6 +1010,9 @@
       <c r="F25" s="7">
         <v>3</v>
       </c>
+      <c r="G25" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
@@ -1006,7 +1042,7 @@
         <v>2</v>
       </c>
       <c r="G27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -1045,7 +1081,7 @@
         <v>56</v>
       </c>
       <c r="E30" s="5">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="F30" s="7">
         <v>3</v>
@@ -1059,7 +1095,7 @@
         <v>56</v>
       </c>
       <c r="E31" s="5">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="F31" s="7">
         <v>3</v>
@@ -1073,13 +1109,13 @@
         <v>56</v>
       </c>
       <c r="E32" s="5">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="F32" s="7">
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>31</v>
       </c>
@@ -1087,13 +1123,13 @@
         <v>56</v>
       </c>
       <c r="E33" s="5">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="F33" s="7">
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>32</v>
       </c>
@@ -1101,13 +1137,13 @@
         <v>56</v>
       </c>
       <c r="E34" s="5">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="F34" s="7">
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>33</v>
       </c>
@@ -1115,13 +1151,13 @@
         <v>56</v>
       </c>
       <c r="E35" s="5">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="F35" s="7">
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>34</v>
       </c>
@@ -1135,7 +1171,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>35</v>
       </c>
@@ -1149,7 +1185,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>36</v>
       </c>
@@ -1162,8 +1198,11 @@
       <c r="F38" s="7">
         <v>3</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G38" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>37</v>
       </c>
@@ -1176,8 +1215,11 @@
       <c r="F39" s="7">
         <v>3</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G39" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>38</v>
       </c>
@@ -1191,7 +1233,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>39</v>
       </c>
@@ -1199,13 +1241,13 @@
         <v>56</v>
       </c>
       <c r="E41" s="5">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="F41" s="7">
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>40</v>
       </c>
@@ -1219,7 +1261,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>41</v>
       </c>
@@ -1227,13 +1269,13 @@
         <v>56</v>
       </c>
       <c r="E43" s="5">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="F43" s="7">
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>42</v>
       </c>
@@ -1241,13 +1283,13 @@
         <v>56</v>
       </c>
       <c r="E44" s="5">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="F44" s="7">
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>43</v>
       </c>
@@ -1261,7 +1303,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>44</v>
       </c>
@@ -1269,13 +1311,13 @@
         <v>56</v>
       </c>
       <c r="E46" s="5">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="F46" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>45</v>
       </c>
@@ -1283,13 +1325,13 @@
         <v>56</v>
       </c>
       <c r="E47" s="5">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="F47" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>46</v>
       </c>
@@ -1297,7 +1339,7 @@
         <v>56</v>
       </c>
       <c r="E48" s="5">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="F48" s="7">
         <v>2</v>
@@ -1311,7 +1353,7 @@
         <v>56</v>
       </c>
       <c r="E49" s="5">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="F49" s="7">
         <v>3</v>
@@ -1330,6 +1372,9 @@
       <c r="F50" s="7">
         <v>2</v>
       </c>
+      <c r="G50" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
@@ -1361,6 +1406,9 @@
       <c r="F52" s="7">
         <v>2</v>
       </c>
+      <c r="G52" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
@@ -1384,7 +1432,7 @@
         <v>56</v>
       </c>
       <c r="E54" s="5">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="F54" s="7">
         <v>2</v>

</xml_diff>